<commit_message>
Update Mapping BRO GMW Events.xlsx
</commit_message>
<xml_diff>
--- a/mappings/Mapping BRO GMW Events.xlsx
+++ b/mappings/Mapping BRO GMW Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://3hydro-my.sharepoint.com/personal/jos_von_asmuth_3hydro_nl/Documents/MATLAB/Menyanthes/Meny_OS/branches/Bron_datamodel/Datamodels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://3hydro-my.sharepoint.com/personal/jos_von_asmuth_3hydro_nl/Documents/MATLAB/Menyanthes/Meny_OS/trunk/Datamodels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{7FA45A96-A3C0-4165-8D39-AC29C64859BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5EC8C6F-9DE2-4BE4-AFA0-20548EC21FCB}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{7FA45A96-A3C0-4165-8D39-AC29C64859BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11C14EC3-AF62-44C9-9963-46FBE249A083}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="99">
   <si>
     <t>Put ingericht</t>
   </si>
@@ -306,16 +306,22 @@
     <t>Verwijderen</t>
   </si>
   <si>
-    <t>Object-UitRegistratie</t>
-  </si>
-  <si>
-    <t>Dit is geen echt bericht, maar loopt via de BRO-servicedesk</t>
-  </si>
-  <si>
-    <t>ObjectUitRegistratie</t>
-  </si>
-  <si>
     <t>Uit registratie</t>
+  </si>
+  <si>
+    <t>Leverancier veranderd</t>
+  </si>
+  <si>
+    <t>leverancierVeranderd</t>
+  </si>
+  <si>
+    <t>BRO_Servicedesk</t>
+  </si>
+  <si>
+    <t>Geen bericht of brondocument, maar actie BRO-servicedesk op verzoek</t>
+  </si>
+  <si>
+    <t>objectUitRegistratie</t>
   </si>
 </sst>
 </file>
@@ -353,7 +359,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -412,8 +418,109 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -423,17 +530,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -443,28 +543,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -473,22 +558,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -504,224 +574,12 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -818,68 +676,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1165,692 +1119,716 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="58.5546875" style="41" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.140625" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="20" t="s">
         <v>69</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="22" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="36"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="12" t="s">
         <v>28</v>
       </c>
       <c r="E3" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="37"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G3" s="24"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="38"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="12" t="s">
         <v>32</v>
       </c>
       <c r="E5" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="37"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G5" s="24"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="38"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="39"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G7" s="26"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="37"/>
-    </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="G8" s="24"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="46" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E10" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="G10" s="37"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G10" s="24"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="7" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="38"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="12" t="s">
         <v>22</v>
       </c>
       <c r="E12" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="37"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G12" s="24"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="38"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G13" s="25"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="37"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="G14" s="24"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="12" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="37"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G15" s="24"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="38"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="G16" s="25"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E17" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="G17" s="37"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="G17" s="24"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="12" t="s">
         <v>52</v>
       </c>
       <c r="E18" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="37"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="G18" s="24"/>
+    </row>
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C20" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D20" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E20" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F20" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="G19" s="38"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="G20" s="25"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B21" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C21" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D21" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="29" t="s">
+      <c r="E21" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F21" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="37"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+      <c r="G21" s="24"/>
+    </row>
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B22" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C22" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="F21" t="s">
-        <v>96</v>
-      </c>
-      <c r="G21" s="37" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+      <c r="G22" s="24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B23" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C23" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G22" s="37"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G23" s="37"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="F23" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="24"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24" s="24"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="37"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
+      <c r="G25" s="24"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B26" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C26" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D26" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E26" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F26" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="G25" s="38"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="G26" s="25"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B27" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C27" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="E27" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F27" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="G26" s="37"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+      <c r="G27" s="24"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B28" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C28" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="29" t="s">
+      <c r="E28" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F28" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="G27" s="37"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="G28" s="24"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B29" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C29" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="29" t="s">
+      <c r="E29" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F29" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="G28" s="37"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="G29" s="24"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B30" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="C30" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="D29" s="34" t="s">
+      <c r="D30" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="31" t="s">
+      <c r="E30" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F30" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="G29" s="38"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="6" t="s">
+      <c r="G30" s="25"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="37"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="6" t="s">
+      <c r="G31" s="24"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="G31" s="37"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="6" t="s">
+      <c r="G32" s="24"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="G32" s="37"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="6" t="s">
+      <c r="G33" s="24"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="G33" s="37"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="6" t="s">
+      <c r="G34" s="24"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="G34" s="37"/>
-    </row>
-    <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="12"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="14" t="s">
+      <c r="G35" s="24"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="9"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="G35" s="40"/>
+      <c r="G36" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>